<commit_message>
NEW: Gate Grid added
</commit_message>
<xml_diff>
--- a/Assets/Internationalization/String_Data.xlsx
+++ b/Assets/Internationalization/String_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Game Projects\Godot Projects\city_of_circling\Assets\Internationalization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Game Projects\city_of_circling\Assets\Internationalization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA893EE4-83C6-4885-B36B-205B47DD75D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D0E06C-56C6-41F4-BD0A-BE84700E0B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-7310" windowWidth="21820" windowHeight="37900" xr2:uid="{08590711-CB36-410F-B5A8-7B8F5AA8D814}"/>
+    <workbookView xWindow="21840" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{08590711-CB36-410F-B5A8-7B8F5AA8D814}"/>
   </bookViews>
   <sheets>
     <sheet name="String_Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t>en</t>
   </si>
@@ -549,6 +549,29 @@
   </si>
   <si>
     <t>FRUIT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXIT_BUTTON</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leave The City</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>出城</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXIT_BUTTON_TOOLTIP</t>
+  </si>
+  <si>
+    <t>一旦出城，将无法返回。你的分数会被立即结算。\n确定要出城吗？</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Once left, you will not be able to return. Your score will be calculated immediately. \nAre you sure you want to leave the city?</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -556,7 +579,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1154,48 +1177,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1211,7 +1234,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1507,20 +1530,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D1D195-E5E8-4810-8E47-E25327235024}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.75" customWidth="1"/>
-    <col min="2" max="2" width="56.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="54.875" customWidth="1"/>
+    <col min="1" max="1" width="36.77734375" customWidth="1"/>
+    <col min="2" max="2" width="56.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -1531,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1542,7 +1565,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -1553,7 +1576,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>150</v>
       </c>
@@ -1564,7 +1587,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>151</v>
       </c>
@@ -1575,7 +1598,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1609,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1597,7 +1620,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1608,7 +1631,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1619,7 +1642,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1630,7 +1653,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1641,7 +1664,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1652,7 +1675,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1663,7 +1686,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1674,7 +1697,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1685,7 +1708,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1696,7 +1719,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1707,7 +1730,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1718,7 +1741,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1729,7 +1752,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1740,7 +1763,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1751,7 +1774,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1762,7 +1785,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1773,7 +1796,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1784,7 +1807,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1795,7 +1818,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1806,7 +1829,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1817,7 +1840,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1828,7 +1851,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -1839,7 +1862,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -1850,7 +1873,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -1861,7 +1884,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -1872,7 +1895,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -1883,7 +1906,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -1894,7 +1917,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -1905,7 +1928,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -1916,7 +1939,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -1927,7 +1950,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -1938,7 +1961,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -1949,7 +1972,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -1960,7 +1983,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>73</v>
       </c>
@@ -1971,124 +1994,146 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="28.5">
-      <c r="A46" t="s">
+    <row r="48" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+    <row r="49" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="28.5">
-      <c r="A48" t="s">
+    <row r="50" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>81</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>85</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>87</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="28.5">
-      <c r="A55" t="s">
+    <row r="57" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NEW: Lots of iterations
</commit_message>
<xml_diff>
--- a/Assets/Internationalization/String_Data.xlsx
+++ b/Assets/Internationalization/String_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Game Projects\Godot Projects\city_of_circling\Assets\Internationalization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4A9074-F9D7-487C-90A4-92956864BA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDFC3AE-2BE5-48FE-A4D2-D041AB22A824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{08590711-CB36-410F-B5A8-7B8F5AA8D814}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="231">
   <si>
     <t>en</t>
   </si>
@@ -28,9 +28,6 @@
     <t>zh</t>
   </si>
   <si>
-    <t>TIME_DAY_HOUR_REFRESH</t>
-  </si>
-  <si>
     <t>AFFAIRS_COUPON</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t>BANANA</t>
   </si>
   <si>
-    <t>BLUE</t>
-  </si>
-  <si>
     <t>DRAW_COUPON</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
     <t>GRAPE</t>
   </si>
   <si>
-    <t>GREEN</t>
-  </si>
-  <si>
     <t>HP_POTION</t>
   </si>
   <si>
@@ -70,18 +61,6 @@
     <t>MYSTERY_BOX</t>
   </si>
   <si>
-    <t>ORANGE</t>
-  </si>
-  <si>
-    <t>PURPLE</t>
-  </si>
-  <si>
-    <t>RAINBOW</t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
     <t>SHOP_REFRESH</t>
   </si>
   <si>
@@ -100,12 +79,6 @@
     <t>WATERMELON</t>
   </si>
   <si>
-    <t>WHITE</t>
-  </si>
-  <si>
-    <t>YELLOW</t>
-  </si>
-  <si>
     <t>FRUIT_PRODUCTION</t>
   </si>
   <si>
@@ -223,16 +196,6 @@
     <t>key</t>
   </si>
   <si>
-    <t>DAY %s\n%s:00\n[font_size=26]Shop refresh in %sh[/font_size]</t>
-  </si>
-  <si>
-    <t>第 %s 天\n%s:00\n[font_size=26]商店将在 %s 小时后刷新[/font_size]</t>
-  </si>
-  <si>
-    <t>事务升级券</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>苹果</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -241,10 +204,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>蓝球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>抽奖券</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -261,18 +220,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>绿球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>生命药水</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>抽奖升级券</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>芒果</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -281,22 +232,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>橙球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>紫球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>彩虹球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>红球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>商店刷新</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -305,14 +240,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>贸易升级券</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>交通升级券</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>自选升级券</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -321,14 +248,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>白球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>黄球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>水果产能+</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -500,18 +419,12 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Affairs Upgrade Coupon</t>
-  </si>
-  <si>
     <t>Apple</t>
   </si>
   <si>
     <t>Banana</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
     <t>Draw Coupon</t>
   </si>
   <si>
@@ -524,62 +437,428 @@
     <t>Grape</t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
     <t>Hp Potion</t>
   </si>
   <si>
-    <t>Lottery Upgrade Coupon</t>
-  </si>
-  <si>
     <t>Mango</t>
   </si>
   <si>
     <t>Mystery Box</t>
   </si>
   <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Purple</t>
-  </si>
-  <si>
-    <t>Rainbow</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
     <t>Shop Refresh</t>
   </si>
   <si>
     <t>Strawberry</t>
   </si>
   <si>
-    <t>Trade Upgrade Coupon</t>
-  </si>
-  <si>
-    <t>Traffic Upgrade Coupon</t>
-  </si>
-  <si>
     <t>Upgrade Coupon Of Your Choice</t>
   </si>
   <si>
     <t>Watermelon</t>
   </si>
   <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Yellow</t>
+    <t>PTS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AFFAIRS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRAFFIC</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Movement</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOTTERY</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luck</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>幸运</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRADE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item Pts</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具点数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIME_REFRESH</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIME_DAY_HOUR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[font_size=26]商店将在 %s 小时后刷新[/font_size]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[font_size=26]Shop refresh in %sh[/font_size]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>第 %s 天\n%02d:00\n</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AFFAIRS_SUPPLY_LV1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AFFAIRS_SUPPLY_LV2</t>
+  </si>
+  <si>
+    <t>AFFAIRS_SUPPLY_LV3</t>
+  </si>
+  <si>
+    <t>AFFAIRS_SUPPLY_LV4</t>
+  </si>
+  <si>
+    <t>AFFAIRS_SUPPLY_LV5</t>
+  </si>
+  <si>
+    <t>TRAFFIC_SUPPLY_LV1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRAFFIC_SUPPLY_LV2</t>
+  </si>
+  <si>
+    <t>TRAFFIC_SUPPLY_LV3</t>
+  </si>
+  <si>
+    <t>TRAFFIC_SUPPLY_LV4</t>
+  </si>
+  <si>
+    <t>TRAFFIC_SUPPLY_LV5</t>
+  </si>
+  <si>
+    <t>TRADE_SUPPLY_LV1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRADE_SUPPLY_LV2</t>
+  </si>
+  <si>
+    <t>TRADE_SUPPLY_LV3</t>
+  </si>
+  <si>
+    <t>TRADE_SUPPLY_LV4</t>
+  </si>
+  <si>
+    <t>TRADE_SUPPLY_LV5</t>
+  </si>
+  <si>
+    <t>LOTTERY_SUPPLY_LV1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOTTERY_SUPPLY_LV2</t>
+  </si>
+  <si>
+    <t>LOTTERY_SUPPLY_LV3</t>
+  </si>
+  <si>
+    <t>LOTTERY_SUPPLY_LV4</t>
+  </si>
+  <si>
+    <t>LOTTERY_SUPPLY_LV5</t>
+  </si>
+  <si>
+    <t>四​叶草</t>
+  </si>
+  <si>
+    <t>​兔脚</t>
+  </si>
+  <si>
+    <t>​骰子​</t>
+  </si>
+  <si>
+    <t>招​财猫​</t>
+  </si>
+  <si>
+    <t>幸​运星​</t>
+  </si>
+  <si>
+    <t>滑板</t>
+  </si>
+  <si>
+    <t>​跳板</t>
+  </si>
+  <si>
+    <t>​火箭​</t>
+  </si>
+  <si>
+    <t>​传送门</t>
+  </si>
+  <si>
+    <r>
+      <t>钩爪</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务罗盘</t>
+  </si>
+  <si>
+    <t>​任务日志​</t>
+  </si>
+  <si>
+    <t>​藏​宝图</t>
+  </si>
+  <si>
+    <t>Battle Pass</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗通行证</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quest Bubble</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务气泡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quest Journal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Treasure Map</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compass</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skateboard</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jump Pad</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grappling Hook</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rocket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Portal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clover</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rabbit's Foot</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dice</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maneki Neko </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lucky Star</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>钱袋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coin Bag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Voucher</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>积分券</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shopping Cart</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>购物车</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menbership Card</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>会员卡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商店</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luck Upgrade Coupon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>幸运升级券</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop Upgrade Coupon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商店升级券</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Movement Upgrade Coupon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动升级券</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quest Upgrade Coupon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务升级券</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>天平</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Balance</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUCCESS_RATE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAY %s\n%02d:00\n</t>
+  </si>
+  <si>
+    <t>%.1f%%\n[font_size=34]SUCCESS RATE[/font_size]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>%.1f%%\n[font_size=34]冒险成功率[/font_size]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHOP_MANUAL_REFRESH</t>
+  </si>
+  <si>
+    <t>shop manual refresh</t>
+  </si>
+  <si>
+    <t>解锁商店刷新</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop rarity +</t>
+  </si>
+  <si>
+    <t>商店道具稀有度+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHOP_RARITY_PLUS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHOP_RARITY_PLUS_DESCRIPTION</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHOP_MANUAL_REFRESH_DESCRIPTION</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商店的货物现在每天可以手动刷新 3 次。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shops can now be manually restocked 3 times per day.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ %s -&gt; + %s\n商品稀有度加成\nLv. %s -&gt; %s / %s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ %s -&gt; + %s\nShop High-Rarity Restock Chance\nLv. %s -&gt; %s / %s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,6 +1018,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1165,7 +1451,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1174,6 +1460,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1530,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D1D195-E5E8-4810-8E47-E25327235024}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1545,7 +1834,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1556,585 +1845,838 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>130</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C13" t="s">
-        <v>75</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>144</v>
+        <v>211</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>151</v>
+        <v>205</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>154</v>
+        <v>207</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>155</v>
+        <v>209</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C31" t="s">
-        <v>93</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>146</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>183</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>31</v>
+        <v>182</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>148</v>
+      </c>
+      <c r="B35" t="s">
+        <v>178</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>185</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="13.5" customHeight="1">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>151</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>39</v>
+        <v>186</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>187</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>153</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>189</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>47</v>
+        <v>196</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>156</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>214</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>132</v>
+        <v>199</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>136</v>
+        <v>197</v>
       </c>
       <c r="C45" t="s">
-        <v>135</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C46" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="28.5">
+        <v>160</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C47" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>110</v>
+        <v>161</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C48" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="28.5">
+        <v>162</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>113</v>
+        <v>193</v>
+      </c>
+      <c r="C50" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>164</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>116</v>
+        <v>194</v>
+      </c>
+      <c r="C51" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>224</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>117</v>
+        <v>222</v>
+      </c>
+      <c r="C54" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>219</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>118</v>
+        <v>220</v>
+      </c>
+      <c r="C55" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>37</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A67" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="28.5">
-      <c r="A57" t="s">
-        <v>65</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>121</v>
+      <c r="B67" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A68" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="28.5">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="28.5">
+      <c r="A73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>47</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>49</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>51</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>53</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="28.5">
+      <c r="A80" t="s">
+        <v>56</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>225</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>226</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C82" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATE: Item Icons added and filled
</commit_message>
<xml_diff>
--- a/Assets/Internationalization/String_Data.xlsx
+++ b/Assets/Internationalization/String_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Game Projects\Godot Projects\city_of_circling\Assets\Internationalization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDFC3AE-2BE5-48FE-A4D2-D041AB22A824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5E2574-C835-4CEF-BA70-7AD89B52DAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{08590711-CB36-410F-B5A8-7B8F5AA8D814}"/>
+    <workbookView xWindow="25490" yWindow="-7310" windowWidth="21820" windowHeight="37900" xr2:uid="{08590711-CB36-410F-B5A8-7B8F5AA8D814}"/>
   </bookViews>
   <sheets>
     <sheet name="String_Data" sheetId="1" r:id="rId1"/>
@@ -595,9 +595,6 @@
   </si>
   <si>
     <t>四​叶草</t>
-  </si>
-  <si>
-    <t>​兔脚</t>
   </si>
   <si>
     <t>​骰子​</t>
@@ -698,10 +695,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Rabbit's Foot</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Dice</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -851,6 +844,14 @@
   </si>
   <si>
     <t>+ %s -&gt; + %s\nShop High-Rarity Restock Chance\nLv. %s -&gt; %s / %s</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crystal Ball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>​水晶球​</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1821,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D1D195-E5E8-4810-8E47-E25327235024}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1848,7 +1849,7 @@
         <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C2" t="s">
         <v>144</v>
@@ -1867,13 +1868,13 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="C4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1958,10 +1959,10 @@
         <v>137</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1969,10 +1970,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2046,10 +2047,10 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2079,10 +2080,10 @@
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2090,10 +2091,10 @@
         <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C25" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2156,10 +2157,10 @@
         <v>145</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2167,10 +2168,10 @@
         <v>146</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2178,10 +2179,10 @@
         <v>147</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2189,10 +2190,10 @@
         <v>148</v>
       </c>
       <c r="B35" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" t="s">
         <v>178</v>
-      </c>
-      <c r="C35" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2200,10 +2201,10 @@
         <v>149</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" t="s">
         <v>180</v>
-      </c>
-      <c r="C36" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2211,10 +2212,10 @@
         <v>150</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="13.5" customHeight="1">
@@ -2225,7 +2226,7 @@
         <v>186</v>
       </c>
       <c r="C38" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2233,10 +2234,10 @@
         <v>152</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C39" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2244,10 +2245,10 @@
         <v>153</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2255,10 +2256,10 @@
         <v>154</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2266,10 +2267,10 @@
         <v>155</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C42" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2277,10 +2278,10 @@
         <v>156</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C43" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2288,10 +2289,10 @@
         <v>157</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C44" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2299,10 +2300,10 @@
         <v>158</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C45" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2310,10 +2311,10 @@
         <v>159</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2321,7 +2322,7 @@
         <v>160</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C47" t="s">
         <v>165</v>
@@ -2332,7 +2333,7 @@
         <v>161</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C48" t="s">
         <v>166</v>
@@ -2343,10 +2344,10 @@
         <v>162</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>192</v>
+        <v>229</v>
       </c>
       <c r="C49" t="s">
-        <v>167</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2354,10 +2355,10 @@
         <v>163</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C50" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2365,32 +2366,32 @@
         <v>164</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C54" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>217</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C55" t="s">
         <v>219</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C55" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2659,24 +2660,24 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
+        <v>224</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="C82" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NEW: finished pts ui and srate ui
</commit_message>
<xml_diff>
--- a/Assets/Internationalization/String_Data.xlsx
+++ b/Assets/Internationalization/String_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Game Projects\Godot Projects\city_of_circling\Assets\Internationalization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5E2574-C835-4CEF-BA70-7AD89B52DAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDE9714-5FAD-44B1-A04B-8AC3BF35C9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="-7310" windowWidth="21820" windowHeight="37900" xr2:uid="{08590711-CB36-410F-B5A8-7B8F5AA8D814}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="234">
   <si>
     <t>en</t>
   </si>
@@ -462,43 +462,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>AFFAIRS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>任务</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Quest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRAFFIC</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Movement</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>移动</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>LOTTERY</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Luck</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>幸运</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRADE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -743,10 +715,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Shop</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Luck Upgrade Coupon</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -852,6 +820,50 @@
   </si>
   <si>
     <t>​水晶球​</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>点数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pts</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PTS_UI</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QUEST</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOVEMENT</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LUCK</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHOP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AFFAIRS_TITLE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRAFFIC_TITLE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOTTERY_TITLE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRADE_TITLE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1820,10 +1832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D1D195-E5E8-4810-8E47-E25327235024}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1846,35 +1858,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1915,769 +1927,780 @@
         <v>127</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>130</v>
+        <v>224</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>230</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>132</v>
+        <v>226</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>231</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>135</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>232</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="C12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C14" t="s">
-        <v>210</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>114</v>
+        <v>201</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>203</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>204</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>121</v>
+        <v>195</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>205</v>
+        <v>122</v>
       </c>
       <c r="C24" t="s">
-        <v>206</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C25" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>145</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C32" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C34" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>148</v>
-      </c>
-      <c r="B35" t="s">
-        <v>177</v>
+        <v>140</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="C35" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>149</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>179</v>
+        <v>141</v>
+      </c>
+      <c r="B36" t="s">
+        <v>170</v>
       </c>
       <c r="C36" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C37" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="13.5" customHeight="1">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="13.5" customHeight="1">
       <c r="A39" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C39" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C40" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C42" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="C43" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C44" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C45" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C46" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C47" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C48" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>229</v>
+        <v>183</v>
       </c>
       <c r="C49" t="s">
-        <v>230</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>191</v>
+        <v>221</v>
       </c>
       <c r="C50" t="s">
-        <v>167</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C51" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>222</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C54" t="s">
-        <v>221</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C55" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>209</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>20</v>
+        <v>210</v>
       </c>
       <c r="C56" t="s">
-        <v>71</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
         <v>37</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A66" t="s">
-        <v>39</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C66" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="C67" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" t="s">
+        <v>108</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A69" t="s">
         <v>111</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
         <v>41</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="28.5">
-      <c r="A71" t="s">
+    <row r="72" spans="1:3" ht="28.5">
+      <c r="A72" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
         <v>43</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="28.5">
-      <c r="A73" t="s">
+    <row r="74" spans="1:3" ht="28.5">
+      <c r="A74" t="s">
         <v>44</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>45</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
         <v>55</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="28.5">
-      <c r="A80" t="s">
+    <row r="81" spans="1:3" ht="28.5">
+      <c r="A81" t="s">
         <v>56</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>223</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>224</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C82" t="s">
-        <v>225</v>
+        <v>215</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>216</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C83" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>